<commit_message>
add state participation analysis and parameter participation analysis--PCS_state_space_analysis.m
</commit_message>
<xml_diff>
--- a/PCS_analysis.xlsx
+++ b/PCS_analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\PCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDA7A4B-AF1A-4AC1-B06D-A00711D8A47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93E785-E0DD-4506-B829-4CAFE5D26FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Real part</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +97,14 @@
   </si>
   <si>
     <t>delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EE11AD-4751-4957-A53D-660D2B6D5C19}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:R2"/>
     </sheetView>
   </sheetViews>
@@ -497,40 +506,40 @@
         <v>-15.89</v>
       </c>
       <c r="G1">
-        <v>-194.74</v>
+        <v>-179.74</v>
       </c>
       <c r="H1">
-        <v>-194.74</v>
+        <v>-179.74</v>
       </c>
       <c r="I1">
-        <v>-178.49</v>
+        <v>-165.53</v>
       </c>
       <c r="J1">
-        <v>-178.49</v>
+        <v>-165.53</v>
       </c>
       <c r="K1">
-        <v>-323.7</v>
+        <v>-344.08</v>
       </c>
       <c r="L1">
-        <v>-323.7</v>
+        <v>-344.08</v>
       </c>
       <c r="M1">
-        <v>-314.45</v>
+        <v>-325.55</v>
       </c>
       <c r="N1">
-        <v>-314.45</v>
+        <v>-325.55</v>
       </c>
       <c r="O1">
-        <v>-8.77</v>
+        <v>-16.329999999999998</v>
       </c>
       <c r="P1">
-        <v>-8.77</v>
+        <v>-16.329999999999998</v>
       </c>
       <c r="Q1">
-        <v>-4.8600000000000003</v>
+        <v>-3.77</v>
       </c>
       <c r="R1">
-        <v>-4.8600000000000003</v>
+        <v>-3.77</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
@@ -550,40 +559,40 @@
         <v>-12.24</v>
       </c>
       <c r="G2">
-        <v>1728.27</v>
+        <v>1803.4</v>
       </c>
       <c r="H2">
-        <v>-1728.27</v>
+        <v>-1803.4</v>
       </c>
       <c r="I2">
-        <v>1630.07</v>
+        <v>1705.36</v>
       </c>
       <c r="J2">
-        <v>-1630.07</v>
+        <v>-1705.36</v>
       </c>
       <c r="K2">
-        <v>244.05</v>
+        <v>240.83</v>
       </c>
       <c r="L2">
-        <v>-244.05</v>
+        <v>-240.83</v>
       </c>
       <c r="M2">
-        <v>235.28</v>
+        <v>226.63</v>
       </c>
       <c r="N2">
-        <v>-235.28</v>
+        <v>-226.63</v>
       </c>
       <c r="O2">
-        <v>42.06</v>
+        <v>36.020000000000003</v>
       </c>
       <c r="P2">
-        <v>-42.06</v>
+        <v>-36.020000000000003</v>
       </c>
       <c r="Q2">
-        <v>7.55</v>
+        <v>11.47</v>
       </c>
       <c r="R2">
-        <v>-7.55</v>
+        <v>-11.47</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
@@ -815,40 +824,40 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>1.145E-2</v>
+        <v>9.6600000000000002E-3</v>
       </c>
       <c r="H7" s="1">
-        <v>1.145E-2</v>
+        <v>9.6600000000000002E-3</v>
       </c>
       <c r="I7" s="1">
-        <v>1.3599999999999999E-2</v>
+        <v>1.1379999999999999E-2</v>
       </c>
       <c r="J7" s="1">
-        <v>1.3599999999999999E-2</v>
+        <v>1.1379999999999999E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>0.33611999999999997</v>
+        <v>0.29782999999999998</v>
       </c>
       <c r="L7" s="1">
-        <v>0.33611999999999997</v>
+        <v>0.29782999999999998</v>
       </c>
       <c r="M7" s="1">
-        <v>0.36085</v>
+        <v>0.33334999999999998</v>
       </c>
       <c r="N7" s="1">
-        <v>0.36085</v>
+        <v>0.33334999999999998</v>
       </c>
       <c r="O7">
-        <v>7.5240000000000001E-2</v>
+        <v>0.13866000000000001</v>
       </c>
       <c r="P7">
-        <v>7.5240000000000001E-2</v>
+        <v>0.13866000000000001</v>
       </c>
       <c r="Q7">
-        <v>3.5200000000000001E-3</v>
+        <v>2.0080000000000001E-2</v>
       </c>
       <c r="R7">
-        <v>3.5200000000000001E-3</v>
+        <v>2.0080000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
@@ -868,40 +877,40 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>1.145E-2</v>
+        <v>9.6600000000000002E-3</v>
       </c>
       <c r="H8" s="1">
-        <v>1.145E-2</v>
+        <v>9.6600000000000002E-3</v>
       </c>
       <c r="I8" s="1">
-        <v>1.3599999999999999E-2</v>
+        <v>1.1379999999999999E-2</v>
       </c>
       <c r="J8" s="1">
-        <v>1.3599999999999999E-2</v>
+        <v>1.1379999999999999E-2</v>
       </c>
       <c r="K8" s="1">
-        <v>0.33609</v>
+        <v>0.29780000000000001</v>
       </c>
       <c r="L8" s="1">
-        <v>0.33609</v>
+        <v>0.29780000000000001</v>
       </c>
       <c r="M8" s="1">
-        <v>0.36087999999999998</v>
+        <v>0.33339000000000002</v>
       </c>
       <c r="N8" s="1">
-        <v>0.36087999999999998</v>
+        <v>0.33339000000000002</v>
       </c>
       <c r="O8">
-        <v>7.5249999999999997E-2</v>
+        <v>0.13877999999999999</v>
       </c>
       <c r="P8">
-        <v>7.5249999999999997E-2</v>
+        <v>0.13877999999999999</v>
       </c>
       <c r="Q8">
-        <v>3.7299999999999998E-3</v>
+        <v>2.0119999999999999E-2</v>
       </c>
       <c r="R8">
-        <v>3.7299999999999998E-3</v>
+        <v>2.0119999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -921,40 +930,40 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>5.6099999999999997E-2</v>
+        <v>4.9029999999999997E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>5.6099999999999997E-2</v>
+        <v>4.9029999999999997E-2</v>
       </c>
       <c r="I9" s="1">
-        <v>5.4390000000000001E-2</v>
+        <v>4.7649999999999998E-2</v>
       </c>
       <c r="J9" s="1">
-        <v>5.4390000000000001E-2</v>
+        <v>4.7649999999999998E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>0.41969000000000001</v>
+        <v>0.43975999999999998</v>
       </c>
       <c r="L9" s="1">
-        <v>0.41969000000000001</v>
+        <v>0.43975999999999998</v>
       </c>
       <c r="M9" s="1">
-        <v>0.41524</v>
+        <v>0.43029000000000001</v>
       </c>
       <c r="N9" s="1">
-        <v>0.41524</v>
+        <v>0.43029000000000001</v>
       </c>
       <c r="O9">
-        <v>9.7999999999999997E-4</v>
+        <v>1.5900000000000001E-3</v>
       </c>
       <c r="P9">
-        <v>9.7999999999999997E-4</v>
+        <v>1.5900000000000001E-3</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
@@ -974,40 +983,40 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>5.6099999999999997E-2</v>
+        <v>4.9029999999999997E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>5.6099999999999997E-2</v>
+        <v>4.9029999999999997E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>5.4390000000000001E-2</v>
+        <v>4.7649999999999998E-2</v>
       </c>
       <c r="J10" s="1">
-        <v>5.4390000000000001E-2</v>
+        <v>4.7649999999999998E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>0.41965999999999998</v>
+        <v>0.43973000000000001</v>
       </c>
       <c r="L10" s="1">
-        <v>0.41965999999999998</v>
+        <v>0.43973000000000001</v>
       </c>
       <c r="M10" s="1">
-        <v>0.41526999999999997</v>
+        <v>0.43032999999999999</v>
       </c>
       <c r="N10" s="1">
-        <v>0.41526999999999997</v>
+        <v>0.43032999999999999</v>
       </c>
       <c r="O10">
-        <v>1.01E-3</v>
+        <v>1.67E-3</v>
       </c>
       <c r="P10">
-        <v>1.01E-3</v>
+        <v>1.67E-3</v>
       </c>
       <c r="Q10">
-        <v>4.0000000000000003E-5</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="R10">
-        <v>4.0000000000000003E-5</v>
+        <v>1.2999999999999999E-4</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
@@ -1027,40 +1036,40 @@
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>0.25927</v>
+        <v>0.23588999999999999</v>
       </c>
       <c r="H11" s="1">
-        <v>0.25927</v>
+        <v>0.23588999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>0.26240999999999998</v>
+        <v>0.23832999999999999</v>
       </c>
       <c r="J11" s="1">
-        <v>0.26240999999999998</v>
+        <v>0.23832999999999999</v>
       </c>
       <c r="K11" s="1">
-        <v>9.7989999999999994E-2</v>
+        <v>0.15562999999999999</v>
       </c>
       <c r="L11" s="1">
-        <v>9.7989999999999994E-2</v>
+        <v>0.15562999999999999</v>
       </c>
       <c r="M11" s="1">
-        <v>8.2780000000000006E-2</v>
+        <v>0.13471</v>
       </c>
       <c r="N11" s="1">
-        <v>8.2780000000000006E-2</v>
+        <v>0.13471</v>
       </c>
       <c r="O11">
-        <v>1.2659999999999999E-2</v>
+        <v>2.137E-2</v>
       </c>
       <c r="P11">
-        <v>1.2659999999999999E-2</v>
+        <v>2.137E-2</v>
       </c>
       <c r="Q11">
-        <v>1.2999999999999999E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
       <c r="R11">
-        <v>1.2999999999999999E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
@@ -1080,40 +1089,40 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>0.25927</v>
+        <v>0.23588999999999999</v>
       </c>
       <c r="H12" s="1">
-        <v>0.25927</v>
+        <v>0.23588999999999999</v>
       </c>
       <c r="I12" s="1">
-        <v>0.26240999999999998</v>
+        <v>0.23832999999999999</v>
       </c>
       <c r="J12" s="1">
-        <v>0.26240999999999998</v>
+        <v>0.23832999999999999</v>
       </c>
       <c r="K12" s="1">
-        <v>9.7989999999999994E-2</v>
+        <v>0.15562999999999999</v>
       </c>
       <c r="L12" s="1">
-        <v>9.7989999999999994E-2</v>
+        <v>0.15562999999999999</v>
       </c>
       <c r="M12" s="1">
-        <v>8.2790000000000002E-2</v>
+        <v>0.13471</v>
       </c>
       <c r="N12" s="1">
-        <v>8.2790000000000002E-2</v>
+        <v>0.13471</v>
       </c>
       <c r="O12">
-        <v>1.2659999999999999E-2</v>
+        <v>2.137E-2</v>
       </c>
       <c r="P12">
-        <v>1.2659999999999999E-2</v>
+        <v>2.137E-2</v>
       </c>
       <c r="Q12">
-        <v>1.2999999999999999E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
       <c r="R12">
-        <v>1.2999999999999999E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
@@ -1133,40 +1142,40 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0.24360000000000001</v>
+        <v>0.24374999999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>0.24360000000000001</v>
+        <v>0.24374999999999999</v>
       </c>
       <c r="I13" s="1">
-        <v>0.24182000000000001</v>
+        <v>0.24202000000000001</v>
       </c>
       <c r="J13" s="1">
-        <v>0.24182000000000001</v>
+        <v>0.24202000000000001</v>
       </c>
       <c r="K13" s="1">
-        <v>1.61E-2</v>
+        <v>1.4710000000000001E-2</v>
       </c>
       <c r="L13" s="1">
-        <v>1.61E-2</v>
+        <v>1.4710000000000001E-2</v>
       </c>
       <c r="M13" s="1">
-        <v>1.3390000000000001E-2</v>
+        <v>1.256E-2</v>
       </c>
       <c r="N13" s="1">
-        <v>1.3390000000000001E-2</v>
+        <v>1.256E-2</v>
       </c>
       <c r="O13">
-        <v>5.1000000000000004E-4</v>
+        <v>8.3000000000000001E-4</v>
       </c>
       <c r="P13">
-        <v>5.1000000000000004E-4</v>
+        <v>8.3000000000000001E-4</v>
       </c>
       <c r="Q13">
-        <v>3.0000000000000001E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="R13">
-        <v>3.0000000000000001E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
@@ -1186,40 +1195,40 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>0.24359</v>
+        <v>0.24374999999999999</v>
       </c>
       <c r="H14" s="1">
-        <v>0.24359</v>
+        <v>0.24374999999999999</v>
       </c>
       <c r="I14" s="1">
-        <v>0.24182000000000001</v>
+        <v>0.24203</v>
       </c>
       <c r="J14" s="1">
-        <v>0.24182000000000001</v>
+        <v>0.24203</v>
       </c>
       <c r="K14" s="1">
-        <v>1.61E-2</v>
+        <v>1.4710000000000001E-2</v>
       </c>
       <c r="L14" s="1">
-        <v>1.61E-2</v>
+        <v>1.4710000000000001E-2</v>
       </c>
       <c r="M14" s="1">
-        <v>1.3390000000000001E-2</v>
+        <v>1.256E-2</v>
       </c>
       <c r="N14" s="1">
-        <v>1.3390000000000001E-2</v>
+        <v>1.256E-2</v>
       </c>
       <c r="O14">
-        <v>5.0000000000000001E-4</v>
+        <v>7.9000000000000001E-4</v>
       </c>
       <c r="P14">
-        <v>5.0000000000000001E-4</v>
+        <v>7.9000000000000001E-4</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>4.0000000000000003E-5</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
@@ -1239,40 +1248,40 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>2.3230000000000001E-2</v>
+        <v>4.2439999999999999E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>2.3230000000000001E-2</v>
+        <v>4.2439999999999999E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>2.3179999999999999E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>2.3179999999999999E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>2.9149999999999999E-2</v>
+        <v>4.9259999999999998E-2</v>
       </c>
       <c r="L15" s="1">
-        <v>2.9149999999999999E-2</v>
+        <v>4.9259999999999998E-2</v>
       </c>
       <c r="M15" s="1">
-        <v>1.7690000000000001E-2</v>
+        <v>3.0880000000000001E-2</v>
       </c>
       <c r="N15" s="1">
-        <v>1.7690000000000001E-2</v>
+        <v>3.0880000000000001E-2</v>
       </c>
       <c r="O15">
-        <v>0.44874000000000003</v>
+        <v>0.40146999999999999</v>
       </c>
       <c r="P15">
-        <v>0.44874000000000003</v>
+        <v>0.40146999999999999</v>
       </c>
       <c r="Q15">
-        <v>2.1440000000000001E-2</v>
+        <v>6.1710000000000001E-2</v>
       </c>
       <c r="R15">
-        <v>2.1440000000000001E-2</v>
+        <v>6.1710000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
@@ -1292,40 +1301,40 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>2.3230000000000001E-2</v>
+        <v>4.2439999999999999E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>2.3230000000000001E-2</v>
+        <v>4.2439999999999999E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>2.3179999999999999E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
       <c r="J16" s="1">
-        <v>2.3179999999999999E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>2.9149999999999999E-2</v>
+        <v>4.9259999999999998E-2</v>
       </c>
       <c r="L16" s="1">
-        <v>2.9149999999999999E-2</v>
+        <v>4.9259999999999998E-2</v>
       </c>
       <c r="M16" s="1">
-        <v>1.7690000000000001E-2</v>
+        <v>3.0880000000000001E-2</v>
       </c>
       <c r="N16" s="1">
-        <v>1.7690000000000001E-2</v>
+        <v>3.0880000000000001E-2</v>
       </c>
       <c r="O16">
-        <v>0.44863999999999998</v>
+        <v>0.40146999999999999</v>
       </c>
       <c r="P16">
-        <v>0.44863999999999998</v>
+        <v>0.40146999999999999</v>
       </c>
       <c r="Q16">
-        <v>2.2669999999999999E-2</v>
+        <v>6.1710000000000001E-2</v>
       </c>
       <c r="R16">
-        <v>2.2669999999999999E-2</v>
+        <v>6.1710000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.4">
@@ -1369,16 +1378,16 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>2.418E-2</v>
+        <v>6.3740000000000005E-2</v>
       </c>
       <c r="P17">
-        <v>2.418E-2</v>
+        <v>6.3740000000000005E-2</v>
       </c>
       <c r="Q17">
-        <v>0.622</v>
+        <v>0.56181000000000003</v>
       </c>
       <c r="R17">
-        <v>0.622</v>
+        <v>0.56181000000000003</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.4">
@@ -1422,16 +1431,16 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>2.3650000000000001E-2</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="P18">
-        <v>2.3650000000000001E-2</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="Q18">
-        <v>0.63275000000000003</v>
+        <v>0.60738000000000003</v>
       </c>
       <c r="R18">
-        <v>0.63275000000000003</v>
+        <v>0.60738000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1439,4 +1448,136 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF57AC2-3434-4FA3-9AC8-65ABD5F13BCE}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>-393.71</v>
+      </c>
+      <c r="D1">
+        <v>-154.09</v>
+      </c>
+      <c r="E1">
+        <v>-15.89</v>
+      </c>
+      <c r="F1">
+        <v>-15.89</v>
+      </c>
+      <c r="G1">
+        <v>-179.74</v>
+      </c>
+      <c r="H1">
+        <v>-179.74</v>
+      </c>
+      <c r="I1">
+        <v>-165.53</v>
+      </c>
+      <c r="J1">
+        <v>-165.53</v>
+      </c>
+      <c r="K1">
+        <v>-344.08</v>
+      </c>
+      <c r="L1">
+        <v>-344.08</v>
+      </c>
+      <c r="M1">
+        <v>-325.55</v>
+      </c>
+      <c r="N1">
+        <v>-325.55</v>
+      </c>
+      <c r="O1">
+        <v>-16.329999999999998</v>
+      </c>
+      <c r="P1">
+        <v>-16.329999999999998</v>
+      </c>
+      <c r="Q1">
+        <v>-3.77</v>
+      </c>
+      <c r="R1">
+        <v>-3.77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>12.24</v>
+      </c>
+      <c r="F2">
+        <v>-12.24</v>
+      </c>
+      <c r="G2">
+        <v>1803.4</v>
+      </c>
+      <c r="H2">
+        <v>-1803.4</v>
+      </c>
+      <c r="I2">
+        <v>1705.36</v>
+      </c>
+      <c r="J2">
+        <v>-1705.36</v>
+      </c>
+      <c r="K2">
+        <v>240.83</v>
+      </c>
+      <c r="L2">
+        <v>-240.83</v>
+      </c>
+      <c r="M2">
+        <v>226.63</v>
+      </c>
+      <c r="N2">
+        <v>-226.63</v>
+      </c>
+      <c r="O2">
+        <v>36.020000000000003</v>
+      </c>
+      <c r="P2">
+        <v>-36.020000000000003</v>
+      </c>
+      <c r="Q2">
+        <v>11.47</v>
+      </c>
+      <c r="R2">
+        <v>-11.47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>